<commit_message>
Enhance timetable generation with academic metrics and column normalization
Update the Python script to normalize column names, identify faculty, duration, and level columns, and calculate total weekly hours and UG/PG session counts for each faculty, storing this in a summary sheet.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 76f898a5-e4b3-4f3c-afb6-5cc69e953a3f
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: 80149a26-9916-4a2d-8f7b-c3bdd02135f0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/e80859ca-dd02-4a58-b26d-d8c7ff296e5c/76f898a5-e4b3-4f3c-afb6-5cc69e953a3f/G5oBZK6
Replit-Helium-Checkpoint-Created: true
</commit_message>
<xml_diff>
--- a/client/public/sample_timetable.xlsx
+++ b/client/public/sample_timetable.xlsx
@@ -14,96 +14,120 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
-  <si>
-    <t>Faculty</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+  <si>
+    <t>Professor Name</t>
+  </si>
+  <si>
+    <t>Course Code</t>
   </si>
   <si>
     <t>Subject</t>
   </si>
   <si>
+    <t>Level (UG/PG)</t>
+  </si>
+  <si>
     <t>Day</t>
   </si>
   <si>
     <t>Time Slot</t>
   </si>
   <si>
+    <t>Duration (Hours)</t>
+  </si>
+  <si>
     <t>Room</t>
   </si>
   <si>
-    <t>Batch</t>
-  </si>
-  <si>
-    <t>John Doe</t>
-  </si>
-  <si>
-    <t>Jane Smith</t>
-  </si>
-  <si>
-    <t>Robert Brown</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
-    <t>Physics</t>
-  </si>
-  <si>
-    <t>Chemistry</t>
-  </si>
-  <si>
-    <t>Biology</t>
-  </si>
-  <si>
-    <t>Computer Science</t>
+    <t>Dr. Alan Turing</t>
+  </si>
+  <si>
+    <t>Prof. Ada Lovelace</t>
+  </si>
+  <si>
+    <t>Dr. Grace Hopper</t>
+  </si>
+  <si>
+    <t>CS101</t>
+  </si>
+  <si>
+    <t>CS302</t>
+  </si>
+  <si>
+    <t>MATH201</t>
+  </si>
+  <si>
+    <t>MATH405</t>
+  </si>
+  <si>
+    <t>CS205</t>
+  </si>
+  <si>
+    <t>Intro to Computing</t>
+  </si>
+  <si>
+    <t>Theory of Computation</t>
+  </si>
+  <si>
+    <t>Discrete Math</t>
+  </si>
+  <si>
+    <t>Advanced Calculus</t>
+  </si>
+  <si>
+    <t>Systems Programming</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>PG</t>
   </si>
   <si>
     <t>Monday</t>
   </si>
   <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
     <t>Tuesday</t>
   </si>
   <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
     <t>Thursday</t>
   </si>
   <si>
     <t>Friday</t>
   </si>
   <si>
-    <t>09:00 - 10:30</t>
-  </si>
-  <si>
-    <t>11:00 - 12:30</t>
-  </si>
-  <si>
-    <t>14:00 - 15:30</t>
-  </si>
-  <si>
-    <t>Room 101</t>
+    <t>09:00-11:00</t>
+  </si>
+  <si>
+    <t>14:00-16:00</t>
+  </si>
+  <si>
+    <t>10:00-12:00</t>
+  </si>
+  <si>
+    <t>11:00-13:00</t>
+  </si>
+  <si>
+    <t>09:00-12:00</t>
+  </si>
+  <si>
+    <t>Auditorium A</t>
+  </si>
+  <si>
+    <t>Lab 4</t>
+  </si>
+  <si>
+    <t>Room 102</t>
+  </si>
+  <si>
+    <t>Room 305</t>
   </si>
   <si>
     <t>Lab 1</t>
-  </si>
-  <si>
-    <t>Room 202</t>
-  </si>
-  <si>
-    <t>Lab 2</t>
-  </si>
-  <si>
-    <t>Lab 3</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>C3</t>
   </si>
 </sst>
 </file>
@@ -435,13 +459,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -460,105 +484,141 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C5" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="F2" t="s">
-        <v>27</v>
+      <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>